<commit_message>
2022-02-22 Tool3 update version2
</commit_message>
<xml_diff>
--- a/data/BordenTool_Data_Template.xlsx
+++ b/data/BordenTool_Data_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmori\Desktop\GSI Work Files\5648_SERDP_Borden\BordenTool_Hannah\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmori\Desktop\GSI Work Files\5648_SERDP_Borden\5648_TA2_Transition_Assessment_Assistant_20210802\5648_TA2-Transition-Assessment-Assistant_1a\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFCDB65-2E0E-4AA6-8A59-58B4B456E043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDA9DBE-8822-49F0-A25C-A4AA001DAE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11835" firstSheet="1" activeTab="3" xr2:uid="{B6BEC480-661E-42A6-BA37-CCE8FD228D15}"/>
+    <workbookView xWindow="31455" yWindow="795" windowWidth="21600" windowHeight="15180" activeTab="2" xr2:uid="{B6BEC480-661E-42A6-BA37-CCE8FD228D15}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Soil_Type</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>1,2-DCA</t>
+  </si>
+  <si>
+    <t>it was 0.47 before</t>
   </si>
 </sst>
 </file>
@@ -769,8 +772,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +821,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.47</v>
+        <v>0.45</v>
       </c>
       <c r="C3">
         <v>1.8731073647818483E-5</v>
@@ -826,6 +829,9 @@
       <c r="D3">
         <f>C3*100/24/60/60</f>
         <v>2.1679483388678803E-8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -843,7 +849,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>